<commit_message>
added img to readme
</commit_message>
<xml_diff>
--- a/MSDS692_Figures_DecoderRing.xlsx
+++ b/MSDS692_Figures_DecoderRing.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9676edfc3f3b3502/Documents/School/_REGIS/2023-08_Fall/MSDS692/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="217" documentId="8_{C7432767-C888-4559-941A-BA8B48197F76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5C84FB5-4869-4F7F-979D-138833948EFA}"/>
+  <xr:revisionPtr revIDLastSave="222" documentId="8_{C7432767-C888-4559-941A-BA8B48197F76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BED37AFE-2D27-4A37-848F-35AC6D0BFFCE}"/>
   <bookViews>
-    <workbookView xWindow="-10845" yWindow="-17250" windowWidth="10860" windowHeight="22110" xr2:uid="{480E1819-0E9A-4256-B878-38D1048C4480}"/>
+    <workbookView xWindow="-15570" yWindow="-17265" windowWidth="15600" windowHeight="19710" xr2:uid="{480E1819-0E9A-4256-B878-38D1048C4480}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1797" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1798" uniqueCount="47">
   <si>
     <t>Description</t>
   </si>
@@ -171,10 +170,13 @@
     <t>Year (YEAR)</t>
   </si>
   <si>
-    <t>entiment-by-Year-of-Presidency-CHRONO</t>
+    <t>Year of Presidency</t>
   </si>
   <si>
-    <t>Year of Presidency</t>
+    <t>Sentiment-by-Year-of-Presidency-CHRONO</t>
+  </si>
+  <si>
+    <t>Keep?</t>
   </si>
 </sst>
 </file>
@@ -530,20 +532,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BFCCC9-89C7-4505-9E64-977EDDE439E8}">
-  <dimension ref="A1:F754"/>
+  <dimension ref="A1:G754"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="3" max="3" width="37.5859375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.29296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.1171875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.1171875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.05859375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -562,8 +565,11 @@
       <c r="F1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="G1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -580,7 +586,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -597,7 +603,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -614,7 +620,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -631,7 +637,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -648,7 +654,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>6</v>
       </c>
@@ -665,7 +671,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>7</v>
       </c>
@@ -682,7 +688,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>8</v>
       </c>
@@ -699,7 +705,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>9</v>
       </c>
@@ -716,7 +722,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A11">
         <v>10</v>
       </c>
@@ -733,7 +739,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A12">
         <v>11</v>
       </c>
@@ -750,7 +756,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A13">
         <v>12</v>
       </c>
@@ -767,7 +773,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A14">
         <v>13</v>
       </c>
@@ -784,7 +790,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A15">
         <v>14</v>
       </c>
@@ -801,7 +807,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A16">
         <v>15</v>
       </c>
@@ -10703,13 +10709,13 @@
         <v>21</v>
       </c>
       <c r="C598" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D598" t="s">
         <v>23</v>
       </c>
       <c r="E598" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="599" spans="1:5" x14ac:dyDescent="0.5">

</xml_diff>